<commit_message>
Locally Weighted Regression Started
</commit_message>
<xml_diff>
--- a/ML001.xlsx
+++ b/ML001.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\ml001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85D1E56-2DF6-4E50-894E-E425BB8D8C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE7664C-C195-4026-894A-418BB992FE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A6D760C-A997-4F73-B650-A0AA2D6E9FA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9A6D760C-A997-4F73-B650-A0AA2D6E9FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="ml0201" sheetId="1" r:id="rId1"/>
+    <sheet name="ml0301" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Height</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -546,6 +547,1387 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6710411198600175E-2"/>
+                  <c:y val="0.30092592592592593"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'ml0301'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'ml0301'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CCF-42CC-AC5B-A62F668BD452}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="457692432"/>
+        <c:axId val="457693088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="457692432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weight</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457693088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="457693088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Height</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457692432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3255249343832018E-2"/>
+                  <c:y val="-3.8253135024788568E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000_);[Red]\(#,##0.000000\)" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'ml0301'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'ml0301'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0AFE-4B65-B06D-283C9E8BD12F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="457692432"/>
+        <c:axId val="457693088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="457692432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weight</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457693088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="457693088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Height</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457692432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3255249343832018E-2"/>
+                  <c:y val="-3.8253135024788568E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000_);[Red]\(#,##0.000000\)" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'ml0301'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'ml0301'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AFF2-4944-B403-50D2F5F88931}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="457692432"/>
+        <c:axId val="457693088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="457692432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weight</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457693088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="457693088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ml0201'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Height</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457692432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId4"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -586,7 +1968,1675 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1141,6 +4191,180 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF1A242E-2920-4EA1-B069-EE410F831047}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB2B3394-E7EC-4B95-9845-4DD197D93AC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B8D644-0339-43D1-9801-912092D92D0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.46345</cdr:x>
+      <cdr:y>0.5383</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.66407</cdr:x>
+      <cdr:y>0.73292</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="直接连接符 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FA0DDCD-B7FF-4F0C-AD69-83E5CF19BDCD}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="2838451" y="2476501"/>
+          <a:ext cx="1228725" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="22225">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1438,12 +4662,584 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F206FE-A4B8-458E-BBC7-409EAA0616D2}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1518,4 +5314,126 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5E825C-E4FA-4FE0-BC8C-F36E619C8790}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>120</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>140</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>160</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>170</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>